<commit_message>
Fixed graph colors so AB is always orange, MCTS is blue
</commit_message>
<xml_diff>
--- a/final_report_data.xlsx
+++ b/final_report_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OSU\AI 531 - Artificial Intelligence\Projects\ai531-mnk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66D4C6EC-255B-4635-8270-E0494586E5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{EF8BE259-5B93-437A-8E6D-BAE901C295EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360"/>
   </bookViews>
@@ -1217,6 +1217,577 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>MCTS (P1) vs. AB (P2)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>scratch_1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MCTS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>scratch_1!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3x3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3x4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4x4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5x4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5x5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6x6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7x7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>scratch_1!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1B97-4EC5-B8C8-5790F0B82443}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>scratch_1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>scratch_1!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3x3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3x4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4x4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5x4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5x5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6x6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7x7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>scratch_1!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>77</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1B97-4EC5-B8C8-5790F0B82443}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1537853999"/>
+        <c:axId val="1310576319"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1537853999"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Board (K=3)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1310576319"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1310576319"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Win Percentage</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1537853999"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>AB (P1) vs. MCTS (P2)</a:t>
             </a:r>
           </a:p>
@@ -1274,7 +1845,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1366,7 +1937,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1753,1149 +2324,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>MCTS (P1) vs. AB (P2)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>scratch_1!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>MCTS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>scratch_1!$A$2:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>3x3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3x4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4x4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5x4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5x5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6x6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7x7</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>scratch_1!$B$2:$B$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>82</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>23</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1B97-4EC5-B8C8-5790F0B82443}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>scratch_1!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>AB</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>scratch_1!$A$2:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>3x3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3x4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4x4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5x4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5x5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6x6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7x7</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>scratch_1!$C$2:$C$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>66</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>72</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>77</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1B97-4EC5-B8C8-5790F0B82443}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="1537853999"/>
-        <c:axId val="1310576319"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1537853999"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Board (K=3)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1310576319"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1310576319"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Win Percentage</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1537853999"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>AB (P1) vs. MCTS (P2)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>scratch_1!$B$15</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>AB</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>scratch_1!$A$16:$A$22</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>3x3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3x4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4x4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5x4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5x5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6x6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7x7</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>scratch_1!$B$16:$B$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>76</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>82</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>94</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-396B-427C-9A65-964F096EA36F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>scratch_1!$C$15</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>MCTS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>scratch_1!$A$16:$A$22</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>3x3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3x4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4x4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5x4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5x5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6x6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7x7</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>scratch_1!$C$16:$C$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-396B-427C-9A65-964F096EA36F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="1987760479"/>
-        <c:axId val="1987754239"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1987760479"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Board (K=3)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1987754239"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1987754239"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Win Percentage</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1987760479"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3509,7 +2938,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4323,46 +3752,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -6428,522 +5817,6 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7499,42 +6372,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>31750</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E6D488F-1125-5C7B-C77A-859358600557}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -7563,6 +6400,42 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DF78201-410E-C33A-7AA2-2C892A7D7990}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
@@ -7572,22 +6445,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:colOff>34926</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>3174</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>542926</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7">
+        <xdr:cNvPr id="9" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DF78201-410E-C33A-7AA2-2C892A7D7990}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B138C5B1-4AAE-C943-AF84-748610FF1396}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7607,52 +6480,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>3175</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>606425</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>1044575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>603250</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B138C5B1-4AAE-C943-AF84-748610FF1396}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>603250</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>1041400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7671,7 +6508,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7980,7 +6817,7 @@
   <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z34" sqref="Z34"/>
+      <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>